<commit_message>
Combined ATACH and ERICH
</commit_message>
<xml_diff>
--- a/ATACH2/ATACH2 PUDS Data Dictionary.xlsx
+++ b/ATACH2/ATACH2 PUDS Data Dictionary.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\Documents\GitHub\ich-laterality\ATACH2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15716F6F-C007-4FFA-8555-3283AE69B4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="60" windowWidth="18645" windowHeight="14520" firstSheet="13" activeTab="23"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form List" sheetId="1" r:id="rId1"/>
@@ -382,9 +388,6 @@
     <t>1 - Left, 2 - Right</t>
   </si>
   <si>
-    <t>F03Q01</t>
-  </si>
-  <si>
     <t>Previous Stroke/TIA</t>
   </si>
   <si>
@@ -2006,12 +2009,15 @@
   </si>
   <si>
     <t>1 - USA, 2 - Japan, 3 - China, 4 - South Korea, 5 - Taiwan, 6 - Germany</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2085,6 +2091,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2132,7 +2141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2165,9 +2174,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2200,6 +2226,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2375,11 +2418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,297 +2433,297 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>573</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B37">
     <sortCondition ref="A2:A37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2689,11 +2732,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,54 +2758,54 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
-      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s">
         <v>190</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" t="s">
         <v>194</v>
-      </c>
-      <c r="B7" t="s">
-        <v>195</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -2770,26 +2813,26 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" t="s">
         <v>196</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>198</v>
-      </c>
-      <c r="B10" t="s">
-        <v>199</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2797,18 +2840,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" t="s">
         <v>200</v>
-      </c>
-      <c r="B12" t="s">
-        <v>201</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -2816,11 +2859,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2846,27 +2890,27 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B3" t="s">
         <v>489</v>
-      </c>
-      <c r="B3" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>491</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>492</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -2874,7 +2918,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
@@ -2885,7 +2929,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -2896,7 +2940,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
@@ -2907,7 +2951,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
@@ -2918,10 +2962,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
         <v>206</v>
-      </c>
-      <c r="B9" t="s">
-        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>69</v>
@@ -2929,10 +2973,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" t="s">
         <v>208</v>
-      </c>
-      <c r="B10" t="s">
-        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -2940,7 +2984,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
@@ -2951,10 +2995,10 @@
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -2963,7 +3007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2990,41 +3034,41 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
         <v>212</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" t="s">
         <v>215</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3033,10 +3077,10 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3059,200 +3103,200 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>494</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -3264,7 +3308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3291,38 +3335,38 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" t="s">
         <v>264</v>
-      </c>
-      <c r="B4" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
         <v>266</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3331,7 +3375,121 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.7109375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>499</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3357,77 +3515,74 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
-      </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>270</v>
+        <v>543</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>273</v>
+        <v>544</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>501</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3435,118 +3590,7 @@
         <v>500</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.7109375" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>286</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>290</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>502</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>501</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3555,7 +3599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3581,27 +3625,27 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B3" t="s">
         <v>504</v>
-      </c>
-      <c r="B3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>506</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>507</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -3609,106 +3653,106 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" t="s">
         <v>296</v>
-      </c>
-      <c r="B5" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" t="s">
         <v>298</v>
-      </c>
-      <c r="B6" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" t="s">
         <v>300</v>
-      </c>
-      <c r="B7" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" t="s">
         <v>302</v>
-      </c>
-      <c r="B8" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" t="s">
         <v>304</v>
-      </c>
-      <c r="B9" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" t="s">
         <v>306</v>
-      </c>
-      <c r="B10" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>307</v>
+      </c>
+      <c r="B11" t="s">
         <v>308</v>
-      </c>
-      <c r="B11" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" t="s">
         <v>310</v>
-      </c>
-      <c r="B12" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" t="s">
         <v>312</v>
-      </c>
-      <c r="B13" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
         <v>314</v>
-      </c>
-      <c r="B14" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15" t="s">
         <v>316</v>
-      </c>
-      <c r="B15" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" t="s">
         <v>318</v>
-      </c>
-      <c r="B16" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B17" t="s">
         <v>320</v>
-      </c>
-      <c r="B17" t="s">
-        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3717,11 +3761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3743,101 +3787,101 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>323</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>338</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>556</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>557</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -3847,7 +3891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3873,35 +3917,35 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" t="s">
         <v>341</v>
-      </c>
-      <c r="B3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" t="s">
         <v>343</v>
-      </c>
-      <c r="B4" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3910,11 +3954,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3936,27 +3980,27 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -3978,7 +4022,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>29</v>
@@ -4000,7 +4044,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4008,7 +4052,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4016,7 +4060,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4024,7 +4068,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4065,7 +4109,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
@@ -4098,7 +4142,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>29</v>
@@ -4109,7 +4153,7 @@
         <v>49</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
@@ -4161,10 +4205,10 @@
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>413</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4172,7 +4216,7 @@
         <v>58</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
@@ -4227,7 +4271,7 @@
         <v>68</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>69</v>
@@ -4238,7 +4282,7 @@
         <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>69</v>
@@ -4260,7 +4304,7 @@
         <v>74</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -4279,7 +4323,7 @@
         <v>78</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>29</v>
@@ -4290,7 +4334,7 @@
         <v>79</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>29</v>
@@ -4301,7 +4345,7 @@
         <v>80</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>29</v>
@@ -4309,18 +4353,18 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>411</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>412</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>29</v>
@@ -4333,7 +4377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4359,41 +4403,41 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4403,7 +4447,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4429,51 +4473,51 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
@@ -4481,29 +4525,29 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
@@ -4511,10 +4555,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>365</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
@@ -4522,18 +4566,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>29</v>
@@ -4541,40 +4585,40 @@
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>525</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>526</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>368</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>29</v>
@@ -4582,10 +4626,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>29</v>
@@ -4593,10 +4637,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
@@ -4604,10 +4648,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>29</v>
@@ -4615,10 +4659,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>29</v>
@@ -4626,10 +4670,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
@@ -4637,10 +4681,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>29</v>
@@ -4648,10 +4692,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>29</v>
@@ -4659,10 +4703,10 @@
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
@@ -4670,10 +4714,10 @@
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>29</v>
@@ -4681,10 +4725,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>29</v>
@@ -4692,10 +4736,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>29</v>
@@ -4703,10 +4747,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>29</v>
@@ -4714,10 +4758,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>29</v>
@@ -4725,10 +4769,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>29</v>
@@ -4736,10 +4780,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>29</v>
@@ -4751,7 +4795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4777,49 +4821,49 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>384</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>29</v>
@@ -4827,18 +4871,18 @@
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>389</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>29</v>
@@ -4846,18 +4890,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
@@ -4865,13 +4909,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>589</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -4880,7 +4924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4906,52 +4950,52 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4960,11 +5004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4986,76 +5030,76 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B3" t="s">
         <v>395</v>
-      </c>
-      <c r="B3" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
         <v>397</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>398</v>
-      </c>
-      <c r="C4" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
         <v>401</v>
-      </c>
-      <c r="C6" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B7" t="s">
         <v>551</v>
-      </c>
-      <c r="B7" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>607</v>
+      </c>
+      <c r="B8" t="s">
         <v>608</v>
-      </c>
-      <c r="B8" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>637</v>
+      </c>
+      <c r="B9" t="s">
         <v>638</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>639</v>
-      </c>
-      <c r="C9" t="s">
-        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -5064,11 +5108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5090,28 +5134,28 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>596</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>29</v>
@@ -5119,97 +5163,97 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -5218,11 +5262,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5244,10 +5288,10 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -5278,7 +5322,7 @@
         <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>29</v>
@@ -5289,7 +5333,7 @@
         <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>29</v>
@@ -5300,7 +5344,7 @@
         <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
@@ -5311,7 +5355,7 @@
         <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>29</v>
@@ -5322,7 +5366,7 @@
         <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>29</v>
@@ -5333,7 +5377,7 @@
         <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
@@ -5345,7 +5389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5372,10 +5416,10 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -5392,34 +5436,34 @@
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5450,11 +5494,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,165 +5520,165 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B3" t="s">
         <v>101</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
-        <v>111</v>
-      </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
         <v>112</v>
       </c>
-      <c r="B8" t="s">
-        <v>113</v>
-      </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
         <v>118</v>
       </c>
-      <c r="B11" t="s">
-        <v>119</v>
-      </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
         <v>122</v>
       </c>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
         <v>124</v>
       </c>
-      <c r="B14" t="s">
-        <v>125</v>
-      </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
         <v>126</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>127</v>
-      </c>
-      <c r="C15" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" t="s">
         <v>129</v>
       </c>
-      <c r="B16" t="s">
-        <v>130</v>
-      </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -5643,11 +5687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5670,19 +5714,19 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -5690,10 +5734,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -5701,10 +5745,10 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -5712,10 +5756,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -5723,10 +5767,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -5734,10 +5778,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
@@ -5745,10 +5789,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -5760,11 +5804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5787,19 +5831,19 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -5807,10 +5851,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -5818,10 +5862,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -5829,10 +5873,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -5840,10 +5884,10 @@
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -5851,10 +5895,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
@@ -5862,10 +5906,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -5873,10 +5917,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -5884,10 +5928,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -5895,10 +5939,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -5906,10 +5950,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -5917,10 +5961,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -5928,77 +5972,77 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" t="s">
         <v>161</v>
-      </c>
-      <c r="C19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -6006,18 +6050,18 @@
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -6025,18 +6069,18 @@
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
@@ -6044,10 +6088,10 @@
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
@@ -6055,10 +6099,10 @@
     </row>
     <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
@@ -6070,7 +6114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6096,94 +6140,94 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
         <v>165</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
         <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
         <v>170</v>
-      </c>
-      <c r="B5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
         <v>172</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
         <v>174</v>
-      </c>
-      <c r="B7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
         <v>176</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" t="s">
         <v>178</v>
-      </c>
-      <c r="B9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" t="s">
         <v>180</v>
-      </c>
-      <c r="B10" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -6191,18 +6235,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B13" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -6214,7 +6258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6240,51 +6284,51 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
         <v>182</v>
-      </c>
-      <c r="B3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
         <v>184</v>
-      </c>
-      <c r="B4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" t="s">
         <v>186</v>
-      </c>
-      <c r="B5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
         <v>188</v>
-      </c>
-      <c r="B6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>